<commit_message>
add feat download war
</commit_message>
<xml_diff>
--- a/service/templates/war-template.xlsx
+++ b/service/templates/war-template.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20403"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I336703\Documents\jabs\ccci\wars-generator\service\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repositories\ccci\war-excel-generate\service\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1BFF85-C5BA-47E1-BA67-00A31827665A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1515973-3F7A-46CF-86E0-DACDBDCABEC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="495" windowWidth="23250" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clockify_Time_Report_Detailed_0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -41,9 +28,6 @@
     <t>Position:</t>
   </si>
   <si>
-    <t>Period Covered:</t>
-  </si>
-  <si>
     <t>Weekly Accomplishment Report</t>
   </si>
   <si>
@@ -71,12 +55,6 @@
     <t>____________________________</t>
   </si>
   <si>
-    <t xml:space="preserve">         ARIEL A. BALITA</t>
-  </si>
-  <si>
-    <t>${table:rows.columns}</t>
-  </si>
-  <si>
     <t>${name}</t>
   </si>
   <si>
@@ -84,13 +62,22 @@
   </si>
   <si>
     <t>${periodCovered}</t>
+  </si>
+  <si>
+    <t>Period Covered</t>
+  </si>
+  <si>
+    <t>ARIEL A. BALITA</t>
+  </si>
+  <si>
+    <t>${table:war.columns}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -112,18 +99,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -132,27 +107,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -167,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -177,51 +146,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -229,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -243,34 +177,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -280,32 +193,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -522,120 +424,117 @@
   <dimension ref="A1:F975"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="90.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="86.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>14</v>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>16</v>
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="9"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="9" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
@@ -1603,11 +1502,6 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:A975">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>